<commit_message>
Modified all .xlsx files.
</commit_message>
<xml_diff>
--- a/Question_1.xlsx
+++ b/Question_1.xlsx
@@ -8,19 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswood/WebstormProjects/Udacity_SQL_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E58AE6FD-7040-A24D-89FF-199A5977817D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D2E92645-658D-774F-9171-470CE3244E3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Question_1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Question_1!$C$2:$C$351</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Question_1!$C$2:$C$351</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Question_1!$C$2:$C$351</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Question_1!$C$2:$C$351</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1646,61 +1640,634 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0">
-      <cx:tx>
-        <cx:txData>
-          <cx:v>Frequency of 'rental_count'</cx:v>
-        </cx:txData>
-      </cx:tx>
-    </cx:title>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="clusteredColumn" uniqueId="{2557981C-F4C3-7E49-A71A-D79B024FFA2C}">
-          <cx:dataPt idx="2"/>
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r">
-              <cx:binSize val="5"/>
-            </cx:binning>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="0.330000013"/>
-        <cx:title>
-          <cx:tx>
-            <cx:txData>
-              <cx:v>rental_count</cx:v>
-            </cx:txData>
-          </cx:tx>
-        </cx:title>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:title>
-          <cx:tx>
-            <cx:txData>
-              <cx:v>Frequency</cx:v>
-            </cx:txData>
-          </cx:tx>
-        </cx:title>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
-    </cx:plotArea>
-  </cx:chart>
-</cx:chartSpace>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>'rental_count' by 'category'</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Total</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>Animation</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Family</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Children</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Comedy</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Classics</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Music</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>1166</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1096</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>945</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>941</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>939</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>830</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C072-1649-A497-110C583C78CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="33"/>
+        <c:overlap val="-30"/>
+        <c:axId val="320648671"/>
+        <c:axId val="1596998127"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="320648671"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>category</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1596998127"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1596998127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>rental_count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="320648671"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst/>
+</c:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1744,7 +2311,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1755,7 +2322,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1778,7 +2345,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -1801,7 +2368,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1809,11 +2376,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -1838,46 +2405,36 @@
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -1892,8 +2449,10 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -1901,12 +2460,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -1916,13 +2472,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1941,38 +2497,41 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2021,6 +2580,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -2052,8 +2617,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2071,8 +2636,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2108,7 +2673,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -2136,18 +2701,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
     <cs:lnRef idx="0"/>
@@ -2157,9 +2711,12 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -2175,7 +2732,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2191,7 +2748,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2205,26 +2762,27 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2238,7 +2796,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -2247,6 +2805,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2256,79 +2820,39 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="2" name="Chart 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07647470-CE46-5E4F-98F0-D5FDAB8C4437}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3136900" y="685800"/>
-              <a:ext cx="9271000" cy="6375400"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4" descr="Chart type: Clustered Bar. 'rental_count' by 'category'&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{131C71AF-A15F-5641-801D-C3EAD360B988}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2634,7 +3158,7 @@
   <dimension ref="A1:C351"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>